<commit_message>
Home Dec Items and pictures(not to size)
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\SEP3-Vibe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7c4ef80be926744/Documents/GitHub/SEP3-Vibe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0350E0-42BB-46A9-B95E-1F86949B0A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="13_ncr:1_{6C0350E0-42BB-46A9-B95E-1F86949B0A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C91FF4-7D62-48DF-BCFD-A1A83FFC6618}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="154">
   <si>
     <t>Stella Drop Earrings</t>
   </si>
@@ -429,12 +429,301 @@
 Pesticide free and reduced water waste
 Vegan</t>
   </si>
+  <si>
+    <t>Forest Floor Wallpaper Mural</t>
+  </si>
+  <si>
+    <t>Misty light filtering through woodland gives off a calming aesthetic and will always be
+ a good choice when looking for a wallpaper that invites a relaxing atmosphere into the 
+space. A perfect choice for a range of spaces but especially well suited to living rooms 
+and bedrooms.</t>
+  </si>
+  <si>
+    <t>*Fire Ratings: European standard en 13501 1 b-s1 d0 &amp; US Standard ASTM e84 fire rating: Class A
+*Install Method: Paste the wall, butt joined
+*Paper Type: non-woven 175 gsm, velvet matte finish
+*Environmental Credentials: PVC-free paper, printed with non-toxic inks and 100% recyclable packaging
+*Made with ethically-sourced PVC-free paper and water-based, non-toxic inks
+*100% plastic-free packaging that's fully recyclable</t>
+  </si>
+  <si>
+    <t>Braid Nook</t>
+  </si>
+  <si>
+    <t>Plaited from a plush wool blend, this petite version of our round Braid rug easily slots 
+into odd-shaped, curved or tight spaces. Assured to age beautifully, its lovely contours 
+restore a sense of calm and comfort into the home.</t>
+  </si>
+  <si>
+    <t>Fiber: Wool viscose blend
+Construction: Hand braided, coiled, stitched
+End finish: N/A
+Height: 3/8" (10 mm)
+78% Wool &amp; 17% Viscose blend, 5% Jute / 100% Cotton Backing</t>
+  </si>
+  <si>
+    <t>Reusable Fabric Gift Wrap 
+Christmas Reindeers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materials - 100% organic cotton fabric, 
+cotton cord and recycled card gift tag, 
+recycled paper wrap guide. </t>
+  </si>
+  <si>
+    <t>These reusable Christmas fabric gift wraps are the ideal zero-waste alternative to 
+wrapping paper. They are made in Britain using organic cotton and can be used over and 
+over again, passed around family and friends and can even be thrown in the washing 
+machine if needed.
+This reusable gift wrapping is printed on organic medium weight cotton and has two cotton braids attached to the corners for easy wrapping.
+A wrapping guide is included with each wrap along as well as a recycled card gift tag for the complete reusable Christmas gift wrapping pack.</t>
+  </si>
+  <si>
+    <t>fabricGiftWrap.png</t>
+  </si>
+  <si>
+    <t>Bamboo Fibre Lunchbox - Pink Coral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bamboo fibre lunchbox with pink coral design with a food grade silicone seal to keep
+ your food fresh and bamboo lid which can be used as a place to put your sandwiches. 
+This environmentally-friendly pack lunchbox is made with sustainable bamboo fibre,
+ corn starch and melamine resin.
+Comes in a blue wave gift box perfect for presents, making it a great eco gift idea. 
+Capacity - 700ml. 
+Care instructions - Dishwasher safe, non microwavable.
+It is not recommended to store liquid in this lunchbox as the wooden lid could swell up. </t>
+  </si>
+  <si>
+    <t>Materials - 50% bamboo, 25% corn starch,
+ 25% melamine resin. 
+Country of Manufacture - china. 
+Product Packaging - Cardboard.</t>
+  </si>
+  <si>
+    <t>Whale Bud Vase Air Plant Holder</t>
+  </si>
+  <si>
+    <t>A handmade ceramic whale, perfect to use as a bud vase or an air plant holder. 
+These little whales are a cheerful piece of home decor with their quirky features and nod 
+to ocean life. Each whale is handcrafted, making every one completely unique. 
+All are glazed inside making them water tight.
+Length: 10cm, Height: 5.2cm, Width: 6cm, Hole Diameter: 2.5cm.
+*Approximate Dimensions.</t>
+  </si>
+  <si>
+    <t>Materials - Stoneware clay.
+Product Packaging - eco friendly packaging.</t>
+  </si>
+  <si>
+    <t>Wildlife Collection Organic Cotton Socks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These statement socks are inspired by Scottish roots.
+Ethically made in Portugal with organic cotton, our original design brings freshness and 
+character to a boring sock drawer.
+</t>
+  </si>
+  <si>
+    <t>Machine wash
+Don’t tumble dry or iron
+78% certified organic cotton, 
+20% polyamide, 2% elastane</t>
+  </si>
+  <si>
+    <t>Birdcage Side Table</t>
+  </si>
+  <si>
+    <t>Materials:
+Recycled Coffee Chaff, 100% Recycled or
+ FSC Certified Birch Ply, Recycled Paper,
+ Non-Toxic Resin, Water-Based and Low
+ VOC Paint, Water-Based Lacquer,
+ Non-Toxic Natural Dye.</t>
+  </si>
+  <si>
+    <t>As a simple side table or a quirky plant stand, this 'birdcage' table is sure to make a 
+statement. The top is made from used coffee bean husk, a byproduct of the coffee 
+roasting industry. The edges have been wrapped in recycled handmade paper, and the 
+legs are made using either recycled birch ply (whenever available) or always FSC certified.
+Table top diametre: 40cm
+Height with legs: 70cm</t>
+  </si>
+  <si>
+    <t>Bamboo Fibre Plate - Dugong</t>
+  </si>
+  <si>
+    <t>These reusable bamboo plates are made with environmentally-friendly bamboo fibre,
+ corn starch and resin, suitable for indoor and outdoor use.
+Great for parties and picnics, they are dishwasher safe and BPA Free.
+Available in a set of 4.
+Size - 22.5cm.</t>
+  </si>
+  <si>
+    <t>Materials - Each item - 50% bamboo fibre,
+ 25% corn starch, 25% melamine binding 
+resin. 
+Product Packaging - Cardboard. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">forestWallpaper.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">braidNookRug.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whaleVase.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildlifeSocks.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birdcageTable.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bambooPlate.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunchBox.png
+</t>
+  </si>
+  <si>
+    <t>RESPIIN MINI JUTE BOWL SET - FIRE</t>
+  </si>
+  <si>
+    <t>A set of three sustainable jute storage nesting bowls in bright red and orange tones made 
+with azo-free dyes. Made from biodegradable and eco-friendly jute, the bowls have a 
+rustic feel with a bright contemporary look, perfect for any environmentally conscious 
+household.
+Large – H6.5 x Dia.16cm
+Medium – H6 x Dia.13.5cm
+Small – H5.5 x Dia.11cm
+Handmade in Bangladesh</t>
+  </si>
+  <si>
+    <t>Recycled Coconut Bowls &amp; Spoons Gift Set</t>
+  </si>
+  <si>
+    <t>Clean U's organic and sustainable Coconut Bowls and Spoons gift set, handmade using reclaimed coconuts that would otherwise be burned after harvest. 
+These sustainable bowls are etched by local craftsmen in the Ben Tre region of Vietnam, each bowl is handpicked from the thickest and highest quality coconuts.
+Available as a set containing - 1x Coconut Bowl &amp; Spoon or 2X Coconut Bowls and 2X Coconut Spoons.
+Care &amp; Usage - Not dishwasher safe. The coconut bowl is not suitable for hot contents due to the natural material.
+Size - Approximately W14cm x H7cm.</t>
+  </si>
+  <si>
+    <t>coconutBowls.png</t>
+  </si>
+  <si>
+    <t>Ingredients - 100% recycled coconut shells 
+and coconut wood. 
+Product packaging - 100% biodegradable 
+cardboard box with recycled shredded 
+coffee cup filler and jute string.</t>
+  </si>
+  <si>
+    <t>juteBowlSet.png</t>
+  </si>
+  <si>
+    <t>Himalayan Salt Candle Holder</t>
+  </si>
+  <si>
+    <t>Harness the benefits of a salt lamp with this 100% natural Himalayan salt tea light holder.
+Provides a warm glow from the candle when lit, creating a lovely relaxing atmosphere. Variation in colour and shape due to the natural beauty of the salt.
+Dimensions (approximately): 9cm Wide, 9cm High.</t>
+  </si>
+  <si>
+    <t>Ingredients - 100% Himalayan Salt. 
+Country of Manufacture - Pakistan. 
+Product Packaging - Recyclable 
+cardboard packaging.</t>
+  </si>
+  <si>
+    <t>candleHolder.png</t>
+  </si>
+  <si>
+    <t>Ceramic Tumbler</t>
+  </si>
+  <si>
+    <t>A unique handmade ceramic tumbler for hot and cold drinks from tea and coffee to water, juice and wine. 
+Crafted by hand, each ceramic cup is hand-thrown of fine stoneware clay and coated with ZAN+ME's own food-safe glazes. The unglazed outer surface enhances the cup’s tactile charm. 
+Care - dishwasher safe, but hand-washing recommended - do not microwave.
+Size - 9.5cm tall x 7.5cm wide. Holds - 200ml. </t>
+  </si>
+  <si>
+    <t>ceramicTumbler.png</t>
+  </si>
+  <si>
+    <t>Materials - High-fired stoneware clay 
+sourced in the UK, in-house glazes. 
+Product Packaging - Recycled paper and 
+cardboard. </t>
+  </si>
+  <si>
+    <t>Breathable Linen Bread Bag</t>
+  </si>
+  <si>
+    <t>This wonderful breathable linen bread bag, featuring a hand printed designs, is ideal for storing loaves, rolls, delicious artisan breads and patisserie. Handmade in Cornwall using natural linen with a cotton tie.
+Measures approx 42cm x 18cm x 12cm.
+Care instructions - Machine washable at 30 degrees.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadBag.png
+</t>
+  </si>
+  <si>
+    <t>Materials - Linen &amp; Cotton. 
+Product Packaging - Paper. 
+Postage Packaging - Brown paper and 
+tissue paper - fully compostable.</t>
+  </si>
+  <si>
+    <t>Recycled Cotton Omar Seat Pad</t>
+  </si>
+  <si>
+    <t>Bring an exotic feel to any indoor or outdoor space with these sustainable seat pads 
+which has been hand crafted with recycled cotton and hand printed using traditional 
+methods from India.
+These intricately patterned seat pads are filled with 100% recycled polyester fibers and are inspired by the mystery of Moroccan windows making them an ideal choice to add a touch of eco-friendly elegance and comfort to any home or garden arrangement.
+Dimensions - 43 x 43cm.</t>
+  </si>
+  <si>
+    <t>Materials - 100% recycled cotton and 
+recycled polyester filling. 
+Product Packaging - Biodegradable cover 
+with Jute and recycled paper tag</t>
+  </si>
+  <si>
+    <t>seatPad.png</t>
+  </si>
+  <si>
+    <t>This gorgeous forest green reusable water bottle reflects the colours of nature whilst also protecting it. Made with recycled, double-walled vacuum-insulated stainless steel keeping cold drinks cold, and hot drinks hot.
+This award-winning Ocean Bottle has an anti-leak dual opening lid, either drink from the bottle or use the lid as a handy drinking cup!
+Size - 500ml.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materials - Stainless steel, BPA-free plastic, silicone rubber and ocean-bound plastic. All materials are fully recyclable. 
+Product Packaging - 100% Recycled and recyclable cardboard box. 
+Plastic free packaging.
+</t>
+  </si>
+  <si>
+    <t>Ocean Bottle - Forest Green</t>
+  </si>
+  <si>
+    <t>oceanBottle.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +736,36 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF403730"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -457,7 +776,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -465,13 +784,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -754,18 +1159,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B91" sqref="B82:B91"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="1" max="1" width="36.77734375" customWidth="1"/>
     <col min="2" max="2" width="72.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" customWidth="1"/>
     <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1023,7 +1428,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -1031,7 +1436,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -1039,7 +1444,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -1047,7 +1452,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -1055,7 +1460,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1063,7 +1468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -1071,7 +1476,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -1079,7 +1484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -1087,7 +1492,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -1095,7 +1500,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>89</v>
       </c>
@@ -1103,7 +1508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -1111,13 +1516,287 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="157.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>93</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>94</v>
       </c>
+    </row>
+    <row r="77" spans="1:5" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E77" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E78" s="8">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="8" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E79" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="8" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E80" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E81" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E82" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E83" s="8">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E84" s="8">
+        <v>9</v>
+      </c>
+      <c r="F84" s="10"/>
+    </row>
+    <row r="85" spans="1:6" s="8" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E85" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="8" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E86" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E87" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E88" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A89" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E89" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E90" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="13" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E91" s="13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="B93" s="2"/>
+    </row>
+    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="B95" s="2"/>
+    </row>
+    <row r="97" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="B97" s="2"/>
+    </row>
+    <row r="99" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="B100" s="2"/>
+    </row>
+    <row r="102" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="B102" s="2"/>
+    </row>
+    <row r="104" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="B104" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
db working, need to add more products
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/802c1c42092691e2/Dokumenty/Uni/SEP/Git/SEP3-Vibe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viaucdk-my.sharepoint.com/personal/315231_viauc_dk/Documents/Dokumenter/GitHub/SEP3-Vibe/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{8307C4C3-7522-4854-8E23-AA87D72026EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB5408AE-1F63-476F-BE92-7E145A25902C}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1181,7 +1181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1227,7 +1227,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1511,11 +1510,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:A411"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.81640625" customWidth="1"/>
     <col min="2" max="2" width="32.453125" customWidth="1"/>
@@ -1526,7 +1525,7 @@
     <col min="8" max="8" width="77.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
         <v>117</v>
@@ -1556,7 +1555,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1678,7 +1677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1736,7 +1735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1794,7 +1793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1852,7 +1851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1968,7 +1967,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="127.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" ht="127.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="118" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" ht="116" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="118" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" ht="116" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2135,7 +2134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2181,7 +2180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="118" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:15" ht="116" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2204,7 +2203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="118" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:15" ht="116" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:15" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2296,7 +2295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="148.25" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="31" spans="1:15" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2365,14 +2364,14 @@
       <c r="H32" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O32">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="59" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2395,14 +2394,14 @@
       <c r="H33" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="I33" s="23" t="s">
+      <c r="I33" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O33">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="134.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:15" ht="134.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2425,14 +2424,14 @@
       <c r="H34" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="I34" s="23" t="s">
+      <c r="I34" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O34">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2455,14 +2454,14 @@
       <c r="H35" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="I35" s="23" t="s">
+      <c r="I35" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O35">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2485,14 +2484,14 @@
       <c r="H36" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="I36" s="23" t="s">
+      <c r="I36" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O36">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="59" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2515,14 +2514,14 @@
       <c r="H37" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="I37" s="23" t="s">
+      <c r="I37" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O37">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2545,14 +2544,14 @@
       <c r="H38" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="I38" s="23" t="s">
+      <c r="I38" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O38">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2575,14 +2574,14 @@
       <c r="H39" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I39" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O39">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2605,14 +2604,14 @@
       <c r="H40" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="I40" s="23" t="s">
+      <c r="I40" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O40">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2635,14 +2634,14 @@
       <c r="H41" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="I41" s="23" t="s">
+      <c r="I41" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O41">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2662,14 +2661,14 @@
       <c r="H42" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="I42" s="23" t="s">
+      <c r="I42" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O42">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2689,14 +2688,14 @@
       <c r="H43" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="I43" s="23" t="s">
+      <c r="I43" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O43">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2716,14 +2715,14 @@
       <c r="H44" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="I44" s="23" t="s">
+      <c r="I44" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2743,14 +2742,14 @@
       <c r="H45" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="I45" s="23" t="s">
+      <c r="I45" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O45">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="89.25" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="46" spans="1:15" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2771,14 +2770,14 @@
       <c r="H46" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="I46" s="23" t="s">
+      <c r="I46" s="19" t="s">
         <v>257</v>
       </c>
       <c r="O46">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2800,14 +2799,14 @@
       <c r="H47" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I47" s="23" t="s">
+      <c r="I47" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O47">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:15" ht="203" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2829,14 +2828,14 @@
       <c r="H48" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I48" s="23" t="s">
+      <c r="I48" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O48">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="191.75" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:15" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2858,14 +2857,14 @@
       <c r="H49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I49" s="23" t="s">
+      <c r="I49" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O49">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:15" ht="203" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2887,14 +2886,14 @@
       <c r="H50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I50" s="23" t="s">
+      <c r="I50" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O50">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:15" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2916,14 +2915,14 @@
       <c r="H51" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I51" s="23" t="s">
+      <c r="I51" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O51">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="147.5" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:15" ht="145" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2945,14 +2944,14 @@
       <c r="H52" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I52" s="23" t="s">
+      <c r="I52" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O52">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:15" ht="174" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2974,14 +2973,14 @@
       <c r="H53" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I53" s="23" t="s">
+      <c r="I53" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O53">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="59" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3003,14 +3002,14 @@
       <c r="H54" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I54" s="23" t="s">
+      <c r="I54" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O54">
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3032,14 +3031,14 @@
       <c r="H55" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I55" s="23" t="s">
+      <c r="I55" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O55">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="177" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:15" ht="174" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3061,14 +3060,14 @@
       <c r="H56" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I56" s="23" t="s">
+      <c r="I56" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O56">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:15" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3090,14 +3089,14 @@
       <c r="H57" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I57" s="23" t="s">
+      <c r="I57" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O57">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3119,14 +3118,14 @@
       <c r="H58" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I58" s="23" t="s">
+      <c r="I58" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O58">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:15" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3148,14 +3147,14 @@
       <c r="H59" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="I59" s="23" t="s">
+      <c r="I59" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O59">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3177,14 +3176,14 @@
       <c r="H60" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I60" s="23" t="s">
+      <c r="I60" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O60">
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:15" ht="203" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3206,57 +3205,57 @@
       <c r="H61" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I61" s="23" t="s">
+      <c r="I61" s="19" t="s">
         <v>258</v>
       </c>
       <c r="O61">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="157.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="77" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:1" ht="157.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77"/>
     </row>
-    <row r="78" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78"/>
     </row>
-    <row r="79" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79"/>
     </row>
-    <row r="80" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80"/>
     </row>
-    <row r="81" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81"/>
     </row>
-    <row r="82" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82"/>
     </row>
-    <row r="83" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83"/>
     </row>
-    <row r="84" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84"/>
     </row>
-    <row r="85" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85"/>
     </row>
-    <row r="86" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86"/>
     </row>
-    <row r="87" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87"/>
     </row>
-    <row r="88" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88"/>
     </row>
-    <row r="89" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89"/>
     </row>
-    <row r="90" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90"/>
     </row>
-    <row r="91" spans="1:1" s="10" customFormat="1" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="91" spans="1:1" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91"/>
     </row>
   </sheetData>

</xml_diff>